<commit_message>
anomaly report: fix path error, delete some params
</commit_message>
<xml_diff>
--- a/data/coyote_data_sample.xlsx
+++ b/data/coyote_data_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elutions-my.sharepoint.com/personal/zfeng0401_elutions_com/Documents/software backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elutions-my.sharepoint.com/personal/zfeng0401_elutions_com/Documents/Github/Data-Processing-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_41E574A88790DE56CF192D11595ED87656CD0503" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F5FFBA-77F5-441C-A1C0-D6D080442F65}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_41E574A88790DE56CF192D11595ED87656CD0503" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACB01AEE-22C0-4728-ABBA-FF5CA7A47FC5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -718,9 +718,13 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" customWidth="1"/>
     <col min="75" max="75" width="24" customWidth="1"/>
     <col min="76" max="76" width="19" customWidth="1"/>
     <col min="77" max="77" width="29.85546875" customWidth="1"/>
+    <col min="102" max="102" width="1" customWidth="1"/>
+    <col min="103" max="103" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" x14ac:dyDescent="0.25">

</xml_diff>